<commit_message>
update van 1 waarde
</commit_message>
<xml_diff>
--- a/beheer van issues/GitHub geregistreerde issues 2020-04-01 v1.7 - publicatie_voorIIMKL_PMKL.xlsx
+++ b/beheer van issues/GitHub geregistreerde issues 2020-04-01 v1.7 - publicatie_voorIIMKL_PMKL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-review\beheer van issues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF70C130-D353-4547-9DDD-DF5F56ED31A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D69F15-8F85-4913-963E-F04CE707CC07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-7680" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{FB381769-38D6-4077-9ECA-0963F4850A5C}"/>
+    <workbookView xWindow="-19320" yWindow="-7680" windowWidth="19440" windowHeight="15000" xr2:uid="{FB381769-38D6-4077-9ECA-0963F4850A5C}"/>
   </bookViews>
   <sheets>
     <sheet name="TCS - 01-04-2020" sheetId="3" r:id="rId1"/>
@@ -2457,7 +2457,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4651,7 +4651,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
@@ -5714,7 +5714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7DF074-1205-4741-901C-DB9CCECBA167}">
   <dimension ref="A1:BB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update GitHub geregistreerde issues 2020-04-01 v1.7 - publicatie_voorIIMKL_PMKL.xlsx
</commit_message>
<xml_diff>
--- a/beheer van issues/GitHub geregistreerde issues 2020-04-01 v1.7 - publicatie_voorIIMKL_PMKL.xlsx
+++ b/beheer van issues/GitHub geregistreerde issues 2020-04-01 v1.7 - publicatie_voorIIMKL_PMKL.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-review\beheer van issues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D69F15-8F85-4913-963E-F04CE707CC07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5857D2D6-48EC-478A-BA7A-5B820459F284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-7680" windowWidth="19440" windowHeight="15000" xr2:uid="{FB381769-38D6-4077-9ECA-0963F4850A5C}"/>
+    <workbookView xWindow="-19320" yWindow="-7680" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{FB381769-38D6-4077-9ECA-0963F4850A5C}"/>
   </bookViews>
   <sheets>
     <sheet name="TCS - 01-04-2020" sheetId="3" r:id="rId1"/>
     <sheet name="IMKL-issues" sheetId="2" r:id="rId2"/>
-    <sheet name="planning" sheetId="4" r:id="rId3"/>
-    <sheet name="Blad1" sheetId="5" r:id="rId4"/>
+    <sheet name="Planning" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'IMKL-issues'!$A$1:$I$1</definedName>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="307">
   <si>
     <t>Nr</t>
   </si>
@@ -1065,12 +1064,6 @@
     <t>aug</t>
   </si>
   <si>
-    <t>sep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okt </t>
-  </si>
-  <si>
     <t>nov</t>
   </si>
   <si>
@@ -1117,9 +1110,6 @@
   </si>
   <si>
     <t>3)Consultatie</t>
-  </si>
-  <si>
-    <t>4)Release candidate</t>
   </si>
   <si>
     <t>5)Vaststellen/publiceren</t>
@@ -1402,7 +1392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1619,131 +1609,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color auto="1"/>
       </left>
@@ -1776,7 +1641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2078,57 +1943,34 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2457,7 +2299,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5406,316 +5248,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D15E0F-0084-4586-B4A9-1ED5E149D483}">
-  <dimension ref="A2:J18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="118"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="102" t="s">
-        <v>280</v>
-      </c>
-      <c r="D2" s="102" t="s">
-        <v>281</v>
-      </c>
-      <c r="E2" s="102" t="s">
-        <v>282</v>
-      </c>
-      <c r="F2" s="102" t="s">
-        <v>283</v>
-      </c>
-      <c r="G2" s="102" t="s">
-        <v>284</v>
-      </c>
-      <c r="H2" s="102" t="s">
-        <v>285</v>
-      </c>
-      <c r="I2" s="102" t="s">
-        <v>286</v>
-      </c>
-      <c r="J2" s="103" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
-        <v>299</v>
-      </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="107"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="120" t="s">
-        <v>300</v>
-      </c>
-      <c r="B4" s="108"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="110"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="119" t="s">
-        <v>301</v>
-      </c>
-      <c r="B5" s="104"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="120" t="s">
-        <v>302</v>
-      </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="110"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="119" t="s">
-        <v>303</v>
-      </c>
-      <c r="B7" s="104"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="107"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="113"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="122" t="s">
-        <v>288</v>
-      </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D9" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="110"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="122" t="s">
-        <v>290</v>
-      </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D10" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="110"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="122" t="s">
-        <v>289</v>
-      </c>
-      <c r="B11" s="114"/>
-      <c r="C11" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D11" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="110"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="122" t="s">
-        <v>292</v>
-      </c>
-      <c r="B12" s="114"/>
-      <c r="C12" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D12" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="110"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="122" t="s">
-        <v>291</v>
-      </c>
-      <c r="B13" s="114"/>
-      <c r="C13" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D13" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="110"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="122" t="s">
-        <v>297</v>
-      </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="109"/>
-      <c r="J14" s="110"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="122" t="s">
-        <v>293</v>
-      </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D15" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="110"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="122" t="s">
-        <v>294</v>
-      </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D16" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="109"/>
-      <c r="J16" s="110"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="122" t="s">
-        <v>295</v>
-      </c>
-      <c r="B17" s="114"/>
-      <c r="C17" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="D17" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="110"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="123" t="s">
-        <v>298</v>
-      </c>
-      <c r="B18" s="115"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116" t="s">
-        <v>296</v>
-      </c>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
-      <c r="G18" s="116"/>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="117"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7DF074-1205-4741-901C-DB9CCECBA167}">
   <dimension ref="A1:BB21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE21" sqref="A1:AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5727,1398 +5264,1398 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A1" s="124"/>
-      <c r="B1" s="124"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="132" t="s">
+      <c r="A1" s="101"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="109" t="s">
         <v>280</v>
       </c>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="132" t="s">
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="109" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="132" t="s">
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="109" t="s">
         <v>282</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="129"/>
-      <c r="P1" s="132" t="s">
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="109" t="s">
         <v>283</v>
       </c>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="129"/>
-      <c r="T1" s="132" t="s">
+      <c r="Q1" s="101"/>
+      <c r="R1" s="101"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="109" t="s">
+        <v>301</v>
+      </c>
+      <c r="U1" s="101"/>
+      <c r="V1" s="101"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="109" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y1" s="101"/>
+      <c r="Z1" s="101"/>
+      <c r="AA1" s="106"/>
+      <c r="AB1" s="109" t="s">
+        <v>284</v>
+      </c>
+      <c r="AC1" s="101"/>
+      <c r="AD1" s="101"/>
+      <c r="AE1" s="106"/>
+      <c r="AF1" s="114" t="s">
+        <v>285</v>
+      </c>
+      <c r="AG1" s="112"/>
+      <c r="AH1" s="112"/>
+      <c r="AI1" s="112"/>
+      <c r="AJ1" s="113"/>
+      <c r="AK1" s="113"/>
+      <c r="AL1" s="113"/>
+      <c r="AM1" s="113"/>
+      <c r="AN1" s="113"/>
+      <c r="AO1" s="113"/>
+      <c r="AP1" s="113"/>
+      <c r="AQ1" s="113"/>
+      <c r="AR1" s="113"/>
+      <c r="AS1" s="113"/>
+      <c r="AT1" s="113"/>
+      <c r="AU1" s="113"/>
+      <c r="AV1" s="113"/>
+      <c r="AW1" s="113"/>
+      <c r="AX1" s="113"/>
+      <c r="AY1" s="113"/>
+      <c r="AZ1" s="113"/>
+      <c r="BA1" s="113"/>
+      <c r="BB1" s="113"/>
+    </row>
+    <row r="2" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="110">
+        <v>1</v>
+      </c>
+      <c r="E2" s="102">
+        <v>2</v>
+      </c>
+      <c r="F2" s="102">
+        <v>3</v>
+      </c>
+      <c r="G2" s="107">
+        <v>4</v>
+      </c>
+      <c r="H2" s="110">
+        <v>1</v>
+      </c>
+      <c r="I2" s="102">
+        <v>2</v>
+      </c>
+      <c r="J2" s="102">
+        <v>3</v>
+      </c>
+      <c r="K2" s="107">
+        <v>4</v>
+      </c>
+      <c r="L2" s="110">
+        <v>1</v>
+      </c>
+      <c r="M2" s="102">
+        <v>2</v>
+      </c>
+      <c r="N2" s="102">
+        <v>3</v>
+      </c>
+      <c r="O2" s="107">
+        <v>4</v>
+      </c>
+      <c r="P2" s="110">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="102">
+        <v>2</v>
+      </c>
+      <c r="R2" s="102">
+        <v>3</v>
+      </c>
+      <c r="S2" s="107">
+        <v>4</v>
+      </c>
+      <c r="T2" s="110">
+        <v>1</v>
+      </c>
+      <c r="U2" s="102">
+        <v>2</v>
+      </c>
+      <c r="V2" s="102">
+        <v>3</v>
+      </c>
+      <c r="W2" s="107">
+        <v>4</v>
+      </c>
+      <c r="X2" s="110">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="102">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="102">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="107">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="110">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="102">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="102">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="107">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="114">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="112">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="112">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="112">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="113"/>
+      <c r="AK2" s="113"/>
+      <c r="AL2" s="113"/>
+      <c r="AM2" s="113"/>
+      <c r="AN2" s="113"/>
+      <c r="AO2" s="113"/>
+      <c r="AP2" s="113"/>
+      <c r="AQ2" s="113"/>
+      <c r="AR2" s="113"/>
+      <c r="AS2" s="113"/>
+      <c r="AT2" s="113"/>
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="113"/>
+      <c r="AY2" s="113"/>
+      <c r="AZ2" s="113"/>
+      <c r="BA2" s="113"/>
+      <c r="BB2" s="113"/>
+    </row>
+    <row r="3" spans="1:54" s="105" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="130" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="133"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="111"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="108"/>
+      <c r="AB3" s="111"/>
+      <c r="AC3" s="104"/>
+      <c r="AD3" s="104"/>
+      <c r="AE3" s="108"/>
+      <c r="AF3" s="114"/>
+      <c r="AG3" s="112"/>
+      <c r="AH3" s="112"/>
+      <c r="AI3" s="112"/>
+      <c r="AJ3" s="113"/>
+      <c r="AK3" s="113"/>
+      <c r="AL3" s="113"/>
+      <c r="AM3" s="113"/>
+      <c r="AN3" s="113"/>
+      <c r="AO3" s="113"/>
+      <c r="AP3" s="113"/>
+      <c r="AQ3" s="113"/>
+      <c r="AR3" s="113"/>
+      <c r="AS3" s="113"/>
+      <c r="AT3" s="113"/>
+      <c r="AU3" s="113"/>
+      <c r="AV3" s="113"/>
+      <c r="AW3" s="113"/>
+      <c r="AX3" s="113"/>
+      <c r="AY3" s="113"/>
+      <c r="AZ3" s="113"/>
+      <c r="BA3" s="113"/>
+      <c r="BB3" s="113"/>
+    </row>
+    <row r="4" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="131" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="132"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="110"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="110"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="107"/>
+      <c r="X4" s="110"/>
+      <c r="Y4" s="102"/>
+      <c r="Z4" s="102"/>
+      <c r="AA4" s="107"/>
+      <c r="AB4" s="110"/>
+      <c r="AC4" s="102"/>
+      <c r="AD4" s="102"/>
+      <c r="AE4" s="107"/>
+      <c r="AF4" s="114"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="113"/>
+      <c r="AK4" s="113"/>
+      <c r="AL4" s="113"/>
+      <c r="AM4" s="113"/>
+      <c r="AN4" s="113"/>
+      <c r="AO4" s="113"/>
+      <c r="AP4" s="113"/>
+      <c r="AQ4" s="113"/>
+      <c r="AR4" s="113"/>
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="113"/>
+      <c r="AU4" s="113"/>
+      <c r="AV4" s="113"/>
+      <c r="AW4" s="113"/>
+      <c r="AX4" s="113"/>
+      <c r="AY4" s="113"/>
+      <c r="AZ4" s="113"/>
+      <c r="BA4" s="113"/>
+      <c r="BB4" s="113"/>
+    </row>
+    <row r="5" spans="1:54" s="105" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="130" t="s">
+        <v>299</v>
+      </c>
+      <c r="B5" s="121"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="122"/>
+      <c r="P5" s="123"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="104"/>
+      <c r="V5" s="104"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="111"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="111"/>
+      <c r="AC5" s="104"/>
+      <c r="AD5" s="104"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="114"/>
+      <c r="AG5" s="112"/>
+      <c r="AH5" s="112"/>
+      <c r="AI5" s="112"/>
+      <c r="AJ5" s="113"/>
+      <c r="AK5" s="113"/>
+      <c r="AL5" s="113"/>
+      <c r="AM5" s="113"/>
+      <c r="AN5" s="113"/>
+      <c r="AO5" s="113"/>
+      <c r="AP5" s="113"/>
+      <c r="AQ5" s="113"/>
+      <c r="AR5" s="113"/>
+      <c r="AS5" s="113"/>
+      <c r="AT5" s="113"/>
+      <c r="AU5" s="113"/>
+      <c r="AV5" s="113"/>
+      <c r="AW5" s="113"/>
+      <c r="AX5" s="113"/>
+      <c r="AY5" s="113"/>
+      <c r="AZ5" s="113"/>
+      <c r="BA5" s="113"/>
+      <c r="BB5" s="113"/>
+    </row>
+    <row r="6" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="131" t="s">
         <v>304</v>
       </c>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="129"/>
-      <c r="X1" s="132" t="s">
+      <c r="B6" s="126"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="110"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="110"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="124"/>
+      <c r="T6" s="125"/>
+      <c r="U6" s="126"/>
+      <c r="V6" s="126"/>
+      <c r="W6" s="107"/>
+      <c r="X6" s="110"/>
+      <c r="Y6" s="102"/>
+      <c r="Z6" s="102"/>
+      <c r="AA6" s="107"/>
+      <c r="AB6" s="110"/>
+      <c r="AC6" s="102"/>
+      <c r="AD6" s="102"/>
+      <c r="AE6" s="107"/>
+      <c r="AF6" s="114"/>
+      <c r="AG6" s="112"/>
+      <c r="AH6" s="112"/>
+      <c r="AI6" s="112"/>
+      <c r="AJ6" s="113"/>
+      <c r="AK6" s="113"/>
+      <c r="AL6" s="113"/>
+      <c r="AM6" s="113"/>
+      <c r="AN6" s="113"/>
+      <c r="AO6" s="113"/>
+      <c r="AP6" s="113"/>
+      <c r="AQ6" s="113"/>
+      <c r="AR6" s="113"/>
+      <c r="AS6" s="113"/>
+      <c r="AT6" s="113"/>
+      <c r="AU6" s="113"/>
+      <c r="AV6" s="113"/>
+      <c r="AW6" s="113"/>
+      <c r="AX6" s="113"/>
+      <c r="AY6" s="113"/>
+      <c r="AZ6" s="113"/>
+      <c r="BA6" s="113"/>
+      <c r="BB6" s="113"/>
+    </row>
+    <row r="7" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="131" t="s">
+        <v>303</v>
+      </c>
+      <c r="B7" s="126"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="110"/>
+      <c r="Q7" s="102"/>
+      <c r="R7" s="102"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="125"/>
+      <c r="U7" s="102"/>
+      <c r="V7" s="102"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="110"/>
+      <c r="Y7" s="102"/>
+      <c r="Z7" s="102"/>
+      <c r="AA7" s="107"/>
+      <c r="AB7" s="110"/>
+      <c r="AC7" s="102"/>
+      <c r="AD7" s="102"/>
+      <c r="AE7" s="107"/>
+      <c r="AF7" s="114"/>
+      <c r="AG7" s="112"/>
+      <c r="AH7" s="112"/>
+      <c r="AI7" s="112"/>
+      <c r="AJ7" s="113"/>
+      <c r="AK7" s="113"/>
+      <c r="AL7" s="113"/>
+      <c r="AM7" s="113"/>
+      <c r="AN7" s="113"/>
+      <c r="AO7" s="113"/>
+      <c r="AP7" s="113"/>
+      <c r="AQ7" s="113"/>
+      <c r="AR7" s="113"/>
+      <c r="AS7" s="113"/>
+      <c r="AT7" s="113"/>
+      <c r="AU7" s="113"/>
+      <c r="AV7" s="113"/>
+      <c r="AW7" s="113"/>
+      <c r="AX7" s="113"/>
+      <c r="AY7" s="113"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="113"/>
+      <c r="BB7" s="113"/>
+    </row>
+    <row r="8" spans="1:54" s="105" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="130" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="129"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="111"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="108"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="104"/>
+      <c r="R8" s="104"/>
+      <c r="S8" s="108"/>
+      <c r="T8" s="111"/>
+      <c r="U8" s="104"/>
+      <c r="V8" s="104"/>
+      <c r="W8" s="127"/>
+      <c r="X8" s="128"/>
+      <c r="Y8" s="129"/>
+      <c r="Z8" s="129"/>
+      <c r="AA8" s="108"/>
+      <c r="AB8" s="111"/>
+      <c r="AC8" s="104"/>
+      <c r="AD8" s="104"/>
+      <c r="AE8" s="108"/>
+      <c r="AF8" s="114"/>
+      <c r="AG8" s="112"/>
+      <c r="AH8" s="112"/>
+      <c r="AI8" s="112"/>
+      <c r="AJ8" s="113"/>
+      <c r="AK8" s="113"/>
+      <c r="AL8" s="113"/>
+      <c r="AM8" s="113"/>
+      <c r="AN8" s="113"/>
+      <c r="AO8" s="113"/>
+      <c r="AP8" s="113"/>
+      <c r="AQ8" s="113"/>
+      <c r="AR8" s="113"/>
+      <c r="AS8" s="113"/>
+      <c r="AT8" s="113"/>
+      <c r="AU8" s="113"/>
+      <c r="AV8" s="113"/>
+      <c r="AW8" s="113"/>
+      <c r="AX8" s="113"/>
+      <c r="AY8" s="113"/>
+      <c r="AZ8" s="113"/>
+      <c r="BA8" s="113"/>
+      <c r="BB8" s="113"/>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A9" s="101"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="101"/>
+      <c r="N9" s="101"/>
+      <c r="O9" s="106"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="101"/>
+      <c r="S9" s="106"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="101"/>
+      <c r="V9" s="101"/>
+      <c r="W9" s="106"/>
+      <c r="X9" s="109"/>
+      <c r="Y9" s="101"/>
+      <c r="Z9" s="101"/>
+      <c r="AA9" s="106"/>
+      <c r="AB9" s="109"/>
+      <c r="AC9" s="101"/>
+      <c r="AD9" s="101"/>
+      <c r="AE9" s="106"/>
+      <c r="AF9" s="114"/>
+      <c r="AG9" s="112"/>
+      <c r="AH9" s="112"/>
+      <c r="AI9" s="112"/>
+      <c r="AJ9" s="113"/>
+      <c r="AK9" s="113"/>
+      <c r="AL9" s="113"/>
+      <c r="AM9" s="113"/>
+      <c r="AN9" s="113"/>
+      <c r="AO9" s="113"/>
+      <c r="AP9" s="113"/>
+      <c r="AQ9" s="113"/>
+      <c r="AR9" s="113"/>
+      <c r="AS9" s="113"/>
+      <c r="AT9" s="113"/>
+      <c r="AU9" s="113"/>
+      <c r="AV9" s="113"/>
+      <c r="AW9" s="113"/>
+      <c r="AX9" s="113"/>
+      <c r="AY9" s="113"/>
+      <c r="AZ9" s="113"/>
+      <c r="BA9" s="113"/>
+      <c r="BB9" s="113"/>
+    </row>
+    <row r="10" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="102" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="102"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="E10" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F10" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G10" s="107"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="107"/>
+      <c r="L10" s="110"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="107"/>
+      <c r="P10" s="110"/>
+      <c r="Q10" s="102"/>
+      <c r="R10" s="102"/>
+      <c r="S10" s="107"/>
+      <c r="T10" s="110"/>
+      <c r="U10" s="102"/>
+      <c r="V10" s="102"/>
+      <c r="W10" s="107"/>
+      <c r="X10" s="110"/>
+      <c r="Y10" s="102"/>
+      <c r="Z10" s="102"/>
+      <c r="AA10" s="107"/>
+      <c r="AB10" s="110"/>
+      <c r="AC10" s="102"/>
+      <c r="AD10" s="102"/>
+      <c r="AE10" s="107"/>
+      <c r="AF10" s="114"/>
+      <c r="AG10" s="112"/>
+      <c r="AH10" s="112"/>
+      <c r="AI10" s="112"/>
+      <c r="AJ10" s="113"/>
+      <c r="AK10" s="113"/>
+      <c r="AL10" s="113"/>
+      <c r="AM10" s="113"/>
+      <c r="AN10" s="113"/>
+      <c r="AO10" s="113"/>
+      <c r="AP10" s="113"/>
+      <c r="AQ10" s="113"/>
+      <c r="AR10" s="113"/>
+      <c r="AS10" s="113"/>
+      <c r="AT10" s="113"/>
+      <c r="AU10" s="113"/>
+      <c r="AV10" s="113"/>
+      <c r="AW10" s="113"/>
+      <c r="AX10" s="113"/>
+      <c r="AY10" s="113"/>
+      <c r="AZ10" s="113"/>
+      <c r="BA10" s="113"/>
+      <c r="BB10" s="113"/>
+    </row>
+    <row r="11" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="102" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" s="102"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G11" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H11" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I11" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J11" s="102"/>
+      <c r="K11" s="107"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="110"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="102"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="110"/>
+      <c r="U11" s="102"/>
+      <c r="V11" s="102"/>
+      <c r="W11" s="107"/>
+      <c r="X11" s="110"/>
+      <c r="Y11" s="102"/>
+      <c r="Z11" s="102"/>
+      <c r="AA11" s="107"/>
+      <c r="AB11" s="110"/>
+      <c r="AC11" s="102"/>
+      <c r="AD11" s="102"/>
+      <c r="AE11" s="107"/>
+      <c r="AF11" s="114"/>
+      <c r="AG11" s="112"/>
+      <c r="AH11" s="112"/>
+      <c r="AI11" s="112"/>
+      <c r="AJ11" s="113"/>
+      <c r="AK11" s="113"/>
+      <c r="AL11" s="113"/>
+      <c r="AM11" s="113"/>
+      <c r="AN11" s="113"/>
+      <c r="AO11" s="113"/>
+      <c r="AP11" s="113"/>
+      <c r="AQ11" s="113"/>
+      <c r="AR11" s="113"/>
+      <c r="AS11" s="113"/>
+      <c r="AT11" s="113"/>
+      <c r="AU11" s="113"/>
+      <c r="AV11" s="113"/>
+      <c r="AW11" s="113"/>
+      <c r="AX11" s="113"/>
+      <c r="AY11" s="113"/>
+      <c r="AZ11" s="113"/>
+      <c r="BA11" s="113"/>
+      <c r="BB11" s="113"/>
+    </row>
+    <row r="12" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="102" t="s">
         <v>305</v>
       </c>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="129"/>
-      <c r="AB1" s="132" t="s">
-        <v>286</v>
-      </c>
-      <c r="AC1" s="124"/>
-      <c r="AD1" s="124"/>
-      <c r="AE1" s="129"/>
-      <c r="AF1" s="137" t="s">
+      <c r="B12" s="102"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G12" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H12" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I12" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J12" s="102"/>
+      <c r="K12" s="107"/>
+      <c r="L12" s="110"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="107"/>
+      <c r="P12" s="110"/>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102"/>
+      <c r="S12" s="107"/>
+      <c r="T12" s="110"/>
+      <c r="U12" s="102"/>
+      <c r="V12" s="102"/>
+      <c r="W12" s="107"/>
+      <c r="X12" s="110"/>
+      <c r="Y12" s="102"/>
+      <c r="Z12" s="102"/>
+      <c r="AA12" s="107"/>
+      <c r="AB12" s="110"/>
+      <c r="AC12" s="102"/>
+      <c r="AD12" s="102"/>
+      <c r="AE12" s="107"/>
+      <c r="AF12" s="114"/>
+      <c r="AG12" s="112"/>
+      <c r="AH12" s="112"/>
+      <c r="AI12" s="112"/>
+      <c r="AJ12" s="113"/>
+      <c r="AK12" s="113"/>
+      <c r="AL12" s="113"/>
+      <c r="AM12" s="113"/>
+      <c r="AN12" s="113"/>
+      <c r="AO12" s="113"/>
+      <c r="AP12" s="113"/>
+      <c r="AQ12" s="113"/>
+      <c r="AR12" s="113"/>
+      <c r="AS12" s="113"/>
+      <c r="AT12" s="113"/>
+      <c r="AU12" s="113"/>
+      <c r="AV12" s="113"/>
+      <c r="AW12" s="113"/>
+      <c r="AX12" s="113"/>
+      <c r="AY12" s="113"/>
+      <c r="AZ12" s="113"/>
+      <c r="BA12" s="113"/>
+      <c r="BB12" s="113"/>
+    </row>
+    <row r="13" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="102" t="s">
         <v>287</v>
       </c>
-      <c r="AG1" s="135"/>
-      <c r="AH1" s="135"/>
-      <c r="AI1" s="135"/>
-      <c r="AJ1" s="136"/>
-      <c r="AK1" s="136"/>
-      <c r="AL1" s="136"/>
-      <c r="AM1" s="136"/>
-      <c r="AN1" s="136"/>
-      <c r="AO1" s="136"/>
-      <c r="AP1" s="136"/>
-      <c r="AQ1" s="136"/>
-      <c r="AR1" s="136"/>
-      <c r="AS1" s="136"/>
-      <c r="AT1" s="136"/>
-      <c r="AU1" s="136"/>
-      <c r="AV1" s="136"/>
-      <c r="AW1" s="136"/>
-      <c r="AX1" s="136"/>
-      <c r="AY1" s="136"/>
-      <c r="AZ1" s="136"/>
-      <c r="BA1" s="136"/>
-      <c r="BB1" s="136"/>
-    </row>
-    <row r="2" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="125"/>
-      <c r="B2" s="125"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="133">
-        <v>1</v>
-      </c>
-      <c r="E2" s="125">
-        <v>2</v>
-      </c>
-      <c r="F2" s="125">
-        <v>3</v>
-      </c>
-      <c r="G2" s="130">
-        <v>4</v>
-      </c>
-      <c r="H2" s="133">
-        <v>1</v>
-      </c>
-      <c r="I2" s="125">
-        <v>2</v>
-      </c>
-      <c r="J2" s="125">
-        <v>3</v>
-      </c>
-      <c r="K2" s="130">
-        <v>4</v>
-      </c>
-      <c r="L2" s="133">
-        <v>1</v>
-      </c>
-      <c r="M2" s="125">
-        <v>2</v>
-      </c>
-      <c r="N2" s="125">
-        <v>3</v>
-      </c>
-      <c r="O2" s="130">
-        <v>4</v>
-      </c>
-      <c r="P2" s="133">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="125">
-        <v>2</v>
-      </c>
-      <c r="R2" s="125">
-        <v>3</v>
-      </c>
-      <c r="S2" s="130">
-        <v>4</v>
-      </c>
-      <c r="T2" s="133">
-        <v>1</v>
-      </c>
-      <c r="U2" s="125">
-        <v>2</v>
-      </c>
-      <c r="V2" s="125">
-        <v>3</v>
-      </c>
-      <c r="W2" s="130">
-        <v>4</v>
-      </c>
-      <c r="X2" s="133">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="125">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="125">
-        <v>3</v>
-      </c>
-      <c r="AA2" s="130">
-        <v>4</v>
-      </c>
-      <c r="AB2" s="133">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="125">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="125">
-        <v>3</v>
-      </c>
-      <c r="AE2" s="130">
-        <v>4</v>
-      </c>
-      <c r="AF2" s="137">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="135">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="135">
-        <v>3</v>
-      </c>
-      <c r="AI2" s="135">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="136"/>
-      <c r="AK2" s="136"/>
-      <c r="AL2" s="136"/>
-      <c r="AM2" s="136"/>
-      <c r="AN2" s="136"/>
-      <c r="AO2" s="136"/>
-      <c r="AP2" s="136"/>
-      <c r="AQ2" s="136"/>
-      <c r="AR2" s="136"/>
-      <c r="AS2" s="136"/>
-      <c r="AT2" s="136"/>
-      <c r="AU2" s="136"/>
-      <c r="AV2" s="136"/>
-      <c r="AW2" s="136"/>
-      <c r="AX2" s="136"/>
-      <c r="AY2" s="136"/>
-      <c r="AZ2" s="136"/>
-      <c r="BA2" s="136"/>
-      <c r="BB2" s="136"/>
-    </row>
-    <row r="3" spans="1:54" s="128" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="153" t="s">
-        <v>299</v>
-      </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="131"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="131"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="127"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="134"/>
-      <c r="U3" s="127"/>
-      <c r="V3" s="127"/>
-      <c r="W3" s="131"/>
-      <c r="X3" s="134"/>
-      <c r="Y3" s="127"/>
-      <c r="Z3" s="127"/>
-      <c r="AA3" s="131"/>
-      <c r="AB3" s="134"/>
-      <c r="AC3" s="127"/>
-      <c r="AD3" s="127"/>
-      <c r="AE3" s="131"/>
-      <c r="AF3" s="137"/>
-      <c r="AG3" s="135"/>
-      <c r="AH3" s="135"/>
-      <c r="AI3" s="135"/>
-      <c r="AJ3" s="136"/>
-      <c r="AK3" s="136"/>
-      <c r="AL3" s="136"/>
-      <c r="AM3" s="136"/>
-      <c r="AN3" s="136"/>
-      <c r="AO3" s="136"/>
-      <c r="AP3" s="136"/>
-      <c r="AQ3" s="136"/>
-      <c r="AR3" s="136"/>
-      <c r="AS3" s="136"/>
-      <c r="AT3" s="136"/>
-      <c r="AU3" s="136"/>
-      <c r="AV3" s="136"/>
-      <c r="AW3" s="136"/>
-      <c r="AX3" s="136"/>
-      <c r="AY3" s="136"/>
-      <c r="AZ3" s="136"/>
-      <c r="BA3" s="136"/>
-      <c r="BB3" s="136"/>
-    </row>
-    <row r="4" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="154" t="s">
-        <v>300</v>
-      </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="133"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="141"/>
-      <c r="K4" s="142"/>
-      <c r="L4" s="143"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="125"/>
-      <c r="O4" s="130"/>
-      <c r="P4" s="133"/>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="130"/>
-      <c r="T4" s="133"/>
-      <c r="U4" s="125"/>
-      <c r="V4" s="125"/>
-      <c r="W4" s="130"/>
-      <c r="X4" s="133"/>
-      <c r="Y4" s="125"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="130"/>
-      <c r="AB4" s="133"/>
-      <c r="AC4" s="125"/>
-      <c r="AD4" s="125"/>
-      <c r="AE4" s="130"/>
-      <c r="AF4" s="137"/>
-      <c r="AG4" s="135"/>
-      <c r="AH4" s="135"/>
-      <c r="AI4" s="135"/>
-      <c r="AJ4" s="136"/>
-      <c r="AK4" s="136"/>
-      <c r="AL4" s="136"/>
-      <c r="AM4" s="136"/>
-      <c r="AN4" s="136"/>
-      <c r="AO4" s="136"/>
-      <c r="AP4" s="136"/>
-      <c r="AQ4" s="136"/>
-      <c r="AR4" s="136"/>
-      <c r="AS4" s="136"/>
-      <c r="AT4" s="136"/>
-      <c r="AU4" s="136"/>
-      <c r="AV4" s="136"/>
-      <c r="AW4" s="136"/>
-      <c r="AX4" s="136"/>
-      <c r="AY4" s="136"/>
-      <c r="AZ4" s="136"/>
-      <c r="BA4" s="136"/>
-      <c r="BB4" s="136"/>
-    </row>
-    <row r="5" spans="1:54" s="128" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="153" t="s">
-        <v>301</v>
-      </c>
-      <c r="B5" s="144"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="134"/>
-      <c r="M5" s="144"/>
-      <c r="N5" s="144"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146"/>
-      <c r="Q5" s="144"/>
-      <c r="R5" s="144"/>
-      <c r="S5" s="131"/>
-      <c r="T5" s="134"/>
-      <c r="U5" s="127"/>
-      <c r="V5" s="127"/>
-      <c r="W5" s="131"/>
-      <c r="X5" s="134"/>
-      <c r="Y5" s="127"/>
-      <c r="Z5" s="127"/>
-      <c r="AA5" s="131"/>
-      <c r="AB5" s="134"/>
-      <c r="AC5" s="127"/>
-      <c r="AD5" s="127"/>
-      <c r="AE5" s="131"/>
-      <c r="AF5" s="137"/>
-      <c r="AG5" s="135"/>
-      <c r="AH5" s="135"/>
-      <c r="AI5" s="135"/>
-      <c r="AJ5" s="136"/>
-      <c r="AK5" s="136"/>
-      <c r="AL5" s="136"/>
-      <c r="AM5" s="136"/>
-      <c r="AN5" s="136"/>
-      <c r="AO5" s="136"/>
-      <c r="AP5" s="136"/>
-      <c r="AQ5" s="136"/>
-      <c r="AR5" s="136"/>
-      <c r="AS5" s="136"/>
-      <c r="AT5" s="136"/>
-      <c r="AU5" s="136"/>
-      <c r="AV5" s="136"/>
-      <c r="AW5" s="136"/>
-      <c r="AX5" s="136"/>
-      <c r="AY5" s="136"/>
-      <c r="AZ5" s="136"/>
-      <c r="BA5" s="136"/>
-      <c r="BB5" s="136"/>
-    </row>
-    <row r="6" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="154" t="s">
-        <v>307</v>
-      </c>
-      <c r="B6" s="149"/>
-      <c r="C6" s="130"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="130"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="125"/>
-      <c r="J6" s="125"/>
-      <c r="K6" s="130"/>
-      <c r="L6" s="133"/>
-      <c r="M6" s="125"/>
-      <c r="N6" s="125"/>
-      <c r="O6" s="130"/>
-      <c r="P6" s="133"/>
-      <c r="Q6" s="125"/>
-      <c r="R6" s="125"/>
-      <c r="S6" s="147"/>
-      <c r="T6" s="148"/>
-      <c r="U6" s="149"/>
-      <c r="V6" s="149"/>
-      <c r="W6" s="130"/>
-      <c r="X6" s="133"/>
-      <c r="Y6" s="125"/>
-      <c r="Z6" s="125"/>
-      <c r="AA6" s="130"/>
-      <c r="AB6" s="133"/>
-      <c r="AC6" s="125"/>
-      <c r="AD6" s="125"/>
-      <c r="AE6" s="130"/>
-      <c r="AF6" s="137"/>
-      <c r="AG6" s="135"/>
-      <c r="AH6" s="135"/>
-      <c r="AI6" s="135"/>
-      <c r="AJ6" s="136"/>
-      <c r="AK6" s="136"/>
-      <c r="AL6" s="136"/>
-      <c r="AM6" s="136"/>
-      <c r="AN6" s="136"/>
-      <c r="AO6" s="136"/>
-      <c r="AP6" s="136"/>
-      <c r="AQ6" s="136"/>
-      <c r="AR6" s="136"/>
-      <c r="AS6" s="136"/>
-      <c r="AT6" s="136"/>
-      <c r="AU6" s="136"/>
-      <c r="AV6" s="136"/>
-      <c r="AW6" s="136"/>
-      <c r="AX6" s="136"/>
-      <c r="AY6" s="136"/>
-      <c r="AZ6" s="136"/>
-      <c r="BA6" s="136"/>
-      <c r="BB6" s="136"/>
-    </row>
-    <row r="7" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="154" t="s">
+      <c r="B13" s="102"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G13" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H13" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I13" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J13" s="102"/>
+      <c r="K13" s="107"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="107"/>
+      <c r="P13" s="110"/>
+      <c r="Q13" s="102"/>
+      <c r="R13" s="102"/>
+      <c r="S13" s="107"/>
+      <c r="T13" s="110"/>
+      <c r="U13" s="102"/>
+      <c r="V13" s="102"/>
+      <c r="W13" s="107"/>
+      <c r="X13" s="110"/>
+      <c r="Y13" s="102"/>
+      <c r="Z13" s="102"/>
+      <c r="AA13" s="107"/>
+      <c r="AB13" s="110"/>
+      <c r="AC13" s="102"/>
+      <c r="AD13" s="102"/>
+      <c r="AE13" s="107"/>
+      <c r="AF13" s="114"/>
+      <c r="AG13" s="112"/>
+      <c r="AH13" s="112"/>
+      <c r="AI13" s="112"/>
+      <c r="AJ13" s="113"/>
+      <c r="AK13" s="113"/>
+      <c r="AL13" s="113"/>
+      <c r="AM13" s="113"/>
+      <c r="AN13" s="113"/>
+      <c r="AO13" s="113"/>
+      <c r="AP13" s="113"/>
+      <c r="AQ13" s="113"/>
+      <c r="AR13" s="113"/>
+      <c r="AS13" s="113"/>
+      <c r="AT13" s="113"/>
+      <c r="AU13" s="113"/>
+      <c r="AV13" s="113"/>
+      <c r="AW13" s="113"/>
+      <c r="AX13" s="113"/>
+      <c r="AY13" s="113"/>
+      <c r="AZ13" s="113"/>
+      <c r="BA13" s="113"/>
+      <c r="BB13" s="113"/>
+    </row>
+    <row r="14" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="102" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14" s="102"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F14" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G14" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H14" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I14" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J14" s="102"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="107"/>
+      <c r="P14" s="110"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="102"/>
+      <c r="S14" s="107"/>
+      <c r="T14" s="110"/>
+      <c r="U14" s="102"/>
+      <c r="V14" s="102"/>
+      <c r="W14" s="107"/>
+      <c r="X14" s="110"/>
+      <c r="Y14" s="102"/>
+      <c r="Z14" s="102"/>
+      <c r="AA14" s="107"/>
+      <c r="AB14" s="110"/>
+      <c r="AC14" s="102"/>
+      <c r="AD14" s="102"/>
+      <c r="AE14" s="107"/>
+      <c r="AF14" s="114"/>
+      <c r="AG14" s="112"/>
+      <c r="AH14" s="112"/>
+      <c r="AI14" s="112"/>
+      <c r="AJ14" s="113"/>
+      <c r="AK14" s="113"/>
+      <c r="AL14" s="113"/>
+      <c r="AM14" s="113"/>
+      <c r="AN14" s="113"/>
+      <c r="AO14" s="113"/>
+      <c r="AP14" s="113"/>
+      <c r="AQ14" s="113"/>
+      <c r="AR14" s="113"/>
+      <c r="AS14" s="113"/>
+      <c r="AT14" s="113"/>
+      <c r="AU14" s="113"/>
+      <c r="AV14" s="113"/>
+      <c r="AW14" s="113"/>
+      <c r="AX14" s="113"/>
+      <c r="AY14" s="113"/>
+      <c r="AZ14" s="113"/>
+      <c r="BA14" s="113"/>
+      <c r="BB14" s="113"/>
+    </row>
+    <row r="15" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="102" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" s="102"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F15" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G15" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H15" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="107"/>
+      <c r="L15" s="110"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="110"/>
+      <c r="Q15" s="102"/>
+      <c r="R15" s="102"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="110"/>
+      <c r="U15" s="102"/>
+      <c r="V15" s="102"/>
+      <c r="W15" s="107"/>
+      <c r="X15" s="110"/>
+      <c r="Y15" s="102"/>
+      <c r="Z15" s="102"/>
+      <c r="AA15" s="107"/>
+      <c r="AB15" s="110"/>
+      <c r="AC15" s="102"/>
+      <c r="AD15" s="102"/>
+      <c r="AE15" s="107"/>
+      <c r="AF15" s="114"/>
+      <c r="AG15" s="112"/>
+      <c r="AH15" s="112"/>
+      <c r="AI15" s="112"/>
+      <c r="AJ15" s="113"/>
+      <c r="AK15" s="113"/>
+      <c r="AL15" s="113"/>
+      <c r="AM15" s="113"/>
+      <c r="AN15" s="113"/>
+      <c r="AO15" s="113"/>
+      <c r="AP15" s="113"/>
+      <c r="AQ15" s="113"/>
+      <c r="AR15" s="113"/>
+      <c r="AS15" s="113"/>
+      <c r="AT15" s="113"/>
+      <c r="AU15" s="113"/>
+      <c r="AV15" s="113"/>
+      <c r="AW15" s="113"/>
+      <c r="AX15" s="113"/>
+      <c r="AY15" s="113"/>
+      <c r="AZ15" s="113"/>
+      <c r="BA15" s="113"/>
+      <c r="BB15" s="113"/>
+    </row>
+    <row r="16" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="102" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" s="102"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F16" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G16" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H16" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I16" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J16" s="102"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="107"/>
+      <c r="P16" s="110"/>
+      <c r="Q16" s="102"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="107"/>
+      <c r="T16" s="110"/>
+      <c r="U16" s="102"/>
+      <c r="V16" s="102"/>
+      <c r="W16" s="107"/>
+      <c r="X16" s="110"/>
+      <c r="Y16" s="102"/>
+      <c r="Z16" s="102"/>
+      <c r="AA16" s="107"/>
+      <c r="AB16" s="110"/>
+      <c r="AC16" s="102"/>
+      <c r="AD16" s="102"/>
+      <c r="AE16" s="107"/>
+      <c r="AF16" s="114"/>
+      <c r="AG16" s="112"/>
+      <c r="AH16" s="112"/>
+      <c r="AI16" s="112"/>
+      <c r="AJ16" s="113"/>
+      <c r="AK16" s="113"/>
+      <c r="AL16" s="113"/>
+      <c r="AM16" s="113"/>
+      <c r="AN16" s="113"/>
+      <c r="AO16" s="113"/>
+      <c r="AP16" s="113"/>
+      <c r="AQ16" s="113"/>
+      <c r="AR16" s="113"/>
+      <c r="AS16" s="113"/>
+      <c r="AT16" s="113"/>
+      <c r="AU16" s="113"/>
+      <c r="AV16" s="113"/>
+      <c r="AW16" s="113"/>
+      <c r="AX16" s="113"/>
+      <c r="AY16" s="113"/>
+      <c r="AZ16" s="113"/>
+      <c r="BA16" s="113"/>
+      <c r="BB16" s="113"/>
+    </row>
+    <row r="17" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="102" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="102"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F17" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G17" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H17" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I17" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J17" s="102"/>
+      <c r="K17" s="107"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="107"/>
+      <c r="P17" s="110"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="107"/>
+      <c r="T17" s="110"/>
+      <c r="U17" s="102"/>
+      <c r="V17" s="102"/>
+      <c r="W17" s="107"/>
+      <c r="X17" s="110"/>
+      <c r="Y17" s="102"/>
+      <c r="Z17" s="102"/>
+      <c r="AA17" s="107"/>
+      <c r="AB17" s="110"/>
+      <c r="AC17" s="102"/>
+      <c r="AD17" s="102"/>
+      <c r="AE17" s="107"/>
+      <c r="AF17" s="114"/>
+      <c r="AG17" s="112"/>
+      <c r="AH17" s="112"/>
+      <c r="AI17" s="112"/>
+      <c r="AJ17" s="113"/>
+      <c r="AK17" s="113"/>
+      <c r="AL17" s="113"/>
+      <c r="AM17" s="113"/>
+      <c r="AN17" s="113"/>
+      <c r="AO17" s="113"/>
+      <c r="AP17" s="113"/>
+      <c r="AQ17" s="113"/>
+      <c r="AR17" s="113"/>
+      <c r="AS17" s="113"/>
+      <c r="AT17" s="113"/>
+      <c r="AU17" s="113"/>
+      <c r="AV17" s="113"/>
+      <c r="AW17" s="113"/>
+      <c r="AX17" s="113"/>
+      <c r="AY17" s="113"/>
+      <c r="AZ17" s="113"/>
+      <c r="BA17" s="113"/>
+      <c r="BB17" s="113"/>
+    </row>
+    <row r="18" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="102" t="s">
         <v>306</v>
       </c>
-      <c r="B7" s="149"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-      <c r="O7" s="130"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="125"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="148"/>
-      <c r="U7" s="125"/>
-      <c r="V7" s="125"/>
-      <c r="W7" s="130"/>
-      <c r="X7" s="133"/>
-      <c r="Y7" s="125"/>
-      <c r="Z7" s="125"/>
-      <c r="AA7" s="130"/>
-      <c r="AB7" s="133"/>
-      <c r="AC7" s="125"/>
-      <c r="AD7" s="125"/>
-      <c r="AE7" s="130"/>
-      <c r="AF7" s="137"/>
-      <c r="AG7" s="135"/>
-      <c r="AH7" s="135"/>
-      <c r="AI7" s="135"/>
-      <c r="AJ7" s="136"/>
-      <c r="AK7" s="136"/>
-      <c r="AL7" s="136"/>
-      <c r="AM7" s="136"/>
-      <c r="AN7" s="136"/>
-      <c r="AO7" s="136"/>
-      <c r="AP7" s="136"/>
-      <c r="AQ7" s="136"/>
-      <c r="AR7" s="136"/>
-      <c r="AS7" s="136"/>
-      <c r="AT7" s="136"/>
-      <c r="AU7" s="136"/>
-      <c r="AV7" s="136"/>
-      <c r="AW7" s="136"/>
-      <c r="AX7" s="136"/>
-      <c r="AY7" s="136"/>
-      <c r="AZ7" s="136"/>
-      <c r="BA7" s="136"/>
-      <c r="BB7" s="136"/>
-    </row>
-    <row r="8" spans="1:54" s="128" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="153" t="s">
-        <v>303</v>
-      </c>
-      <c r="B8" s="152"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
-      <c r="K8" s="131"/>
-      <c r="L8" s="134"/>
-      <c r="M8" s="127"/>
-      <c r="N8" s="127"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="134"/>
-      <c r="Q8" s="127"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="131"/>
-      <c r="T8" s="134"/>
-      <c r="U8" s="127"/>
-      <c r="V8" s="127"/>
-      <c r="W8" s="150"/>
-      <c r="X8" s="151"/>
-      <c r="Y8" s="152"/>
-      <c r="Z8" s="152"/>
-      <c r="AA8" s="131"/>
-      <c r="AB8" s="134"/>
-      <c r="AC8" s="127"/>
-      <c r="AD8" s="127"/>
-      <c r="AE8" s="131"/>
-      <c r="AF8" s="137"/>
-      <c r="AG8" s="135"/>
-      <c r="AH8" s="135"/>
-      <c r="AI8" s="135"/>
-      <c r="AJ8" s="136"/>
-      <c r="AK8" s="136"/>
-      <c r="AL8" s="136"/>
-      <c r="AM8" s="136"/>
-      <c r="AN8" s="136"/>
-      <c r="AO8" s="136"/>
-      <c r="AP8" s="136"/>
-      <c r="AQ8" s="136"/>
-      <c r="AR8" s="136"/>
-      <c r="AS8" s="136"/>
-      <c r="AT8" s="136"/>
-      <c r="AU8" s="136"/>
-      <c r="AV8" s="136"/>
-      <c r="AW8" s="136"/>
-      <c r="AX8" s="136"/>
-      <c r="AY8" s="136"/>
-      <c r="AZ8" s="136"/>
-      <c r="BA8" s="136"/>
-      <c r="BB8" s="136"/>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="124"/>
-      <c r="B9" s="124"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="129"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="129"/>
-      <c r="L9" s="132"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="129"/>
-      <c r="P9" s="132"/>
-      <c r="Q9" s="124"/>
-      <c r="R9" s="124"/>
-      <c r="S9" s="129"/>
-      <c r="T9" s="132"/>
-      <c r="U9" s="124"/>
-      <c r="V9" s="124"/>
-      <c r="W9" s="129"/>
-      <c r="X9" s="132"/>
-      <c r="Y9" s="124"/>
-      <c r="Z9" s="124"/>
-      <c r="AA9" s="129"/>
-      <c r="AB9" s="132"/>
-      <c r="AC9" s="124"/>
-      <c r="AD9" s="124"/>
-      <c r="AE9" s="129"/>
-      <c r="AF9" s="137"/>
-      <c r="AG9" s="135"/>
-      <c r="AH9" s="135"/>
-      <c r="AI9" s="135"/>
-      <c r="AJ9" s="136"/>
-      <c r="AK9" s="136"/>
-      <c r="AL9" s="136"/>
-      <c r="AM9" s="136"/>
-      <c r="AN9" s="136"/>
-      <c r="AO9" s="136"/>
-      <c r="AP9" s="136"/>
-      <c r="AQ9" s="136"/>
-      <c r="AR9" s="136"/>
-      <c r="AS9" s="136"/>
-      <c r="AT9" s="136"/>
-      <c r="AU9" s="136"/>
-      <c r="AV9" s="136"/>
-      <c r="AW9" s="136"/>
-      <c r="AX9" s="136"/>
-      <c r="AY9" s="136"/>
-      <c r="AZ9" s="136"/>
-      <c r="BA9" s="136"/>
-      <c r="BB9" s="136"/>
-    </row>
-    <row r="10" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="125" t="s">
-        <v>288</v>
-      </c>
-      <c r="B10" s="125"/>
-      <c r="C10" s="130"/>
-      <c r="D10" s="133" t="s">
+      <c r="B18" s="102"/>
+      <c r="C18" s="107"/>
+      <c r="D18" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="E18" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F18" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G18" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H18" s="110"/>
+      <c r="I18" s="102"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="107"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="102"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="107"/>
+      <c r="P18" s="110"/>
+      <c r="Q18" s="102"/>
+      <c r="R18" s="102"/>
+      <c r="S18" s="107"/>
+      <c r="T18" s="110"/>
+      <c r="U18" s="102"/>
+      <c r="V18" s="102"/>
+      <c r="W18" s="107"/>
+      <c r="X18" s="110"/>
+      <c r="Y18" s="102"/>
+      <c r="Z18" s="102"/>
+      <c r="AA18" s="107"/>
+      <c r="AB18" s="110"/>
+      <c r="AC18" s="102"/>
+      <c r="AD18" s="102"/>
+      <c r="AE18" s="107"/>
+      <c r="AF18" s="114"/>
+      <c r="AG18" s="112"/>
+      <c r="AH18" s="112"/>
+      <c r="AI18" s="112"/>
+      <c r="AJ18" s="113"/>
+      <c r="AK18" s="113"/>
+      <c r="AL18" s="113"/>
+      <c r="AM18" s="113"/>
+      <c r="AN18" s="113"/>
+      <c r="AO18" s="113"/>
+      <c r="AP18" s="113"/>
+      <c r="AQ18" s="113"/>
+      <c r="AR18" s="113"/>
+      <c r="AS18" s="113"/>
+      <c r="AT18" s="113"/>
+      <c r="AU18" s="113"/>
+      <c r="AV18" s="113"/>
+      <c r="AW18" s="113"/>
+      <c r="AX18" s="113"/>
+      <c r="AY18" s="113"/>
+      <c r="AZ18" s="113"/>
+      <c r="BA18" s="113"/>
+      <c r="BB18" s="113"/>
+    </row>
+    <row r="19" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="102" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19" s="102"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F19" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G19" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H19" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I19" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J19" s="102"/>
+      <c r="K19" s="107"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="102"/>
+      <c r="O19" s="107"/>
+      <c r="P19" s="110"/>
+      <c r="Q19" s="102"/>
+      <c r="R19" s="102"/>
+      <c r="S19" s="107"/>
+      <c r="T19" s="110"/>
+      <c r="U19" s="102"/>
+      <c r="V19" s="102"/>
+      <c r="W19" s="107"/>
+      <c r="X19" s="110"/>
+      <c r="Y19" s="102"/>
+      <c r="Z19" s="102"/>
+      <c r="AA19" s="107"/>
+      <c r="AB19" s="110"/>
+      <c r="AC19" s="102"/>
+      <c r="AD19" s="102"/>
+      <c r="AE19" s="107"/>
+      <c r="AF19" s="114"/>
+      <c r="AG19" s="112"/>
+      <c r="AH19" s="112"/>
+      <c r="AI19" s="112"/>
+      <c r="AJ19" s="113"/>
+      <c r="AK19" s="113"/>
+      <c r="AL19" s="113"/>
+      <c r="AM19" s="113"/>
+      <c r="AN19" s="113"/>
+      <c r="AO19" s="113"/>
+      <c r="AP19" s="113"/>
+      <c r="AQ19" s="113"/>
+      <c r="AR19" s="113"/>
+      <c r="AS19" s="113"/>
+      <c r="AT19" s="113"/>
+      <c r="AU19" s="113"/>
+      <c r="AV19" s="113"/>
+      <c r="AW19" s="113"/>
+      <c r="AX19" s="113"/>
+      <c r="AY19" s="113"/>
+      <c r="AZ19" s="113"/>
+      <c r="BA19" s="113"/>
+      <c r="BB19" s="113"/>
+    </row>
+    <row r="20" spans="1:54" s="103" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="102" t="s">
+        <v>293</v>
+      </c>
+      <c r="B20" s="102"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="F20" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="G20" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="H20" s="110" t="s">
+        <v>294</v>
+      </c>
+      <c r="I20" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J20" s="102"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="107"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="102"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="107"/>
+      <c r="T20" s="110"/>
+      <c r="U20" s="102"/>
+      <c r="V20" s="102"/>
+      <c r="W20" s="107"/>
+      <c r="X20" s="110"/>
+      <c r="Y20" s="102"/>
+      <c r="Z20" s="102"/>
+      <c r="AA20" s="107"/>
+      <c r="AB20" s="110"/>
+      <c r="AC20" s="102"/>
+      <c r="AD20" s="102"/>
+      <c r="AE20" s="107"/>
+      <c r="AF20" s="114"/>
+      <c r="AG20" s="112"/>
+      <c r="AH20" s="112"/>
+      <c r="AI20" s="112"/>
+      <c r="AJ20" s="113"/>
+      <c r="AK20" s="113"/>
+      <c r="AL20" s="113"/>
+      <c r="AM20" s="113"/>
+      <c r="AN20" s="113"/>
+      <c r="AO20" s="113"/>
+      <c r="AP20" s="113"/>
+      <c r="AQ20" s="113"/>
+      <c r="AR20" s="113"/>
+      <c r="AS20" s="113"/>
+      <c r="AT20" s="113"/>
+      <c r="AU20" s="113"/>
+      <c r="AV20" s="113"/>
+      <c r="AW20" s="113"/>
+      <c r="AX20" s="113"/>
+      <c r="AY20" s="113"/>
+      <c r="AZ20" s="113"/>
+      <c r="BA20" s="113"/>
+      <c r="BB20" s="113"/>
+    </row>
+    <row r="21" spans="1:54" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="102" t="s">
         <v>296</v>
       </c>
-      <c r="E10" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F10" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G10" s="130"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
-      <c r="K10" s="130"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="125"/>
-      <c r="N10" s="125"/>
-      <c r="O10" s="130"/>
-      <c r="P10" s="133"/>
-      <c r="Q10" s="125"/>
-      <c r="R10" s="125"/>
-      <c r="S10" s="130"/>
-      <c r="T10" s="133"/>
-      <c r="U10" s="125"/>
-      <c r="V10" s="125"/>
-      <c r="W10" s="130"/>
-      <c r="X10" s="133"/>
-      <c r="Y10" s="125"/>
-      <c r="Z10" s="125"/>
-      <c r="AA10" s="130"/>
-      <c r="AB10" s="133"/>
-      <c r="AC10" s="125"/>
-      <c r="AD10" s="125"/>
-      <c r="AE10" s="130"/>
-      <c r="AF10" s="137"/>
-      <c r="AG10" s="135"/>
-      <c r="AH10" s="135"/>
-      <c r="AI10" s="135"/>
-      <c r="AJ10" s="136"/>
-      <c r="AK10" s="136"/>
-      <c r="AL10" s="136"/>
-      <c r="AM10" s="136"/>
-      <c r="AN10" s="136"/>
-      <c r="AO10" s="136"/>
-      <c r="AP10" s="136"/>
-      <c r="AQ10" s="136"/>
-      <c r="AR10" s="136"/>
-      <c r="AS10" s="136"/>
-      <c r="AT10" s="136"/>
-      <c r="AU10" s="136"/>
-      <c r="AV10" s="136"/>
-      <c r="AW10" s="136"/>
-      <c r="AX10" s="136"/>
-      <c r="AY10" s="136"/>
-      <c r="AZ10" s="136"/>
-      <c r="BA10" s="136"/>
-      <c r="BB10" s="136"/>
-    </row>
-    <row r="11" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="125" t="s">
-        <v>290</v>
-      </c>
-      <c r="B11" s="125"/>
-      <c r="C11" s="130"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G11" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H11" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I11" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J11" s="125"/>
-      <c r="K11" s="130"/>
-      <c r="L11" s="133"/>
-      <c r="M11" s="125"/>
-      <c r="N11" s="125"/>
-      <c r="O11" s="130"/>
-      <c r="P11" s="133"/>
-      <c r="Q11" s="125"/>
-      <c r="R11" s="125"/>
-      <c r="S11" s="130"/>
-      <c r="T11" s="133"/>
-      <c r="U11" s="125"/>
-      <c r="V11" s="125"/>
-      <c r="W11" s="130"/>
-      <c r="X11" s="133"/>
-      <c r="Y11" s="125"/>
-      <c r="Z11" s="125"/>
-      <c r="AA11" s="130"/>
-      <c r="AB11" s="133"/>
-      <c r="AC11" s="125"/>
-      <c r="AD11" s="125"/>
-      <c r="AE11" s="130"/>
-      <c r="AF11" s="137"/>
-      <c r="AG11" s="135"/>
-      <c r="AH11" s="135"/>
-      <c r="AI11" s="135"/>
-      <c r="AJ11" s="136"/>
-      <c r="AK11" s="136"/>
-      <c r="AL11" s="136"/>
-      <c r="AM11" s="136"/>
-      <c r="AN11" s="136"/>
-      <c r="AO11" s="136"/>
-      <c r="AP11" s="136"/>
-      <c r="AQ11" s="136"/>
-      <c r="AR11" s="136"/>
-      <c r="AS11" s="136"/>
-      <c r="AT11" s="136"/>
-      <c r="AU11" s="136"/>
-      <c r="AV11" s="136"/>
-      <c r="AW11" s="136"/>
-      <c r="AX11" s="136"/>
-      <c r="AY11" s="136"/>
-      <c r="AZ11" s="136"/>
-      <c r="BA11" s="136"/>
-      <c r="BB11" s="136"/>
-    </row>
-    <row r="12" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="125" t="s">
-        <v>308</v>
-      </c>
-      <c r="B12" s="125"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G12" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H12" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I12" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J12" s="125"/>
-      <c r="K12" s="130"/>
-      <c r="L12" s="133"/>
-      <c r="M12" s="125"/>
-      <c r="N12" s="125"/>
-      <c r="O12" s="130"/>
-      <c r="P12" s="133"/>
-      <c r="Q12" s="125"/>
-      <c r="R12" s="125"/>
-      <c r="S12" s="130"/>
-      <c r="T12" s="133"/>
-      <c r="U12" s="125"/>
-      <c r="V12" s="125"/>
-      <c r="W12" s="130"/>
-      <c r="X12" s="133"/>
-      <c r="Y12" s="125"/>
-      <c r="Z12" s="125"/>
-      <c r="AA12" s="130"/>
-      <c r="AB12" s="133"/>
-      <c r="AC12" s="125"/>
-      <c r="AD12" s="125"/>
-      <c r="AE12" s="130"/>
-      <c r="AF12" s="137"/>
-      <c r="AG12" s="135"/>
-      <c r="AH12" s="135"/>
-      <c r="AI12" s="135"/>
-      <c r="AJ12" s="136"/>
-      <c r="AK12" s="136"/>
-      <c r="AL12" s="136"/>
-      <c r="AM12" s="136"/>
-      <c r="AN12" s="136"/>
-      <c r="AO12" s="136"/>
-      <c r="AP12" s="136"/>
-      <c r="AQ12" s="136"/>
-      <c r="AR12" s="136"/>
-      <c r="AS12" s="136"/>
-      <c r="AT12" s="136"/>
-      <c r="AU12" s="136"/>
-      <c r="AV12" s="136"/>
-      <c r="AW12" s="136"/>
-      <c r="AX12" s="136"/>
-      <c r="AY12" s="136"/>
-      <c r="AZ12" s="136"/>
-      <c r="BA12" s="136"/>
-      <c r="BB12" s="136"/>
-    </row>
-    <row r="13" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="125" t="s">
-        <v>289</v>
-      </c>
-      <c r="B13" s="125"/>
-      <c r="C13" s="130"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F13" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G13" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H13" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I13" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J13" s="125"/>
-      <c r="K13" s="130"/>
-      <c r="L13" s="133"/>
-      <c r="M13" s="125"/>
-      <c r="N13" s="125"/>
-      <c r="O13" s="130"/>
-      <c r="P13" s="133"/>
-      <c r="Q13" s="125"/>
-      <c r="R13" s="125"/>
-      <c r="S13" s="130"/>
-      <c r="T13" s="133"/>
-      <c r="U13" s="125"/>
-      <c r="V13" s="125"/>
-      <c r="W13" s="130"/>
-      <c r="X13" s="133"/>
-      <c r="Y13" s="125"/>
-      <c r="Z13" s="125"/>
-      <c r="AA13" s="130"/>
-      <c r="AB13" s="133"/>
-      <c r="AC13" s="125"/>
-      <c r="AD13" s="125"/>
-      <c r="AE13" s="130"/>
-      <c r="AF13" s="137"/>
-      <c r="AG13" s="135"/>
-      <c r="AH13" s="135"/>
-      <c r="AI13" s="135"/>
-      <c r="AJ13" s="136"/>
-      <c r="AK13" s="136"/>
-      <c r="AL13" s="136"/>
-      <c r="AM13" s="136"/>
-      <c r="AN13" s="136"/>
-      <c r="AO13" s="136"/>
-      <c r="AP13" s="136"/>
-      <c r="AQ13" s="136"/>
-      <c r="AR13" s="136"/>
-      <c r="AS13" s="136"/>
-      <c r="AT13" s="136"/>
-      <c r="AU13" s="136"/>
-      <c r="AV13" s="136"/>
-      <c r="AW13" s="136"/>
-      <c r="AX13" s="136"/>
-      <c r="AY13" s="136"/>
-      <c r="AZ13" s="136"/>
-      <c r="BA13" s="136"/>
-      <c r="BB13" s="136"/>
-    </row>
-    <row r="14" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="125" t="s">
-        <v>292</v>
-      </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F14" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G14" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H14" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I14" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J14" s="125"/>
-      <c r="K14" s="130"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="125"/>
-      <c r="N14" s="125"/>
-      <c r="O14" s="130"/>
-      <c r="P14" s="133"/>
-      <c r="Q14" s="125"/>
-      <c r="R14" s="125"/>
-      <c r="S14" s="130"/>
-      <c r="T14" s="133"/>
-      <c r="U14" s="125"/>
-      <c r="V14" s="125"/>
-      <c r="W14" s="130"/>
-      <c r="X14" s="133"/>
-      <c r="Y14" s="125"/>
-      <c r="Z14" s="125"/>
-      <c r="AA14" s="130"/>
-      <c r="AB14" s="133"/>
-      <c r="AC14" s="125"/>
-      <c r="AD14" s="125"/>
-      <c r="AE14" s="130"/>
-      <c r="AF14" s="137"/>
-      <c r="AG14" s="135"/>
-      <c r="AH14" s="135"/>
-      <c r="AI14" s="135"/>
-      <c r="AJ14" s="136"/>
-      <c r="AK14" s="136"/>
-      <c r="AL14" s="136"/>
-      <c r="AM14" s="136"/>
-      <c r="AN14" s="136"/>
-      <c r="AO14" s="136"/>
-      <c r="AP14" s="136"/>
-      <c r="AQ14" s="136"/>
-      <c r="AR14" s="136"/>
-      <c r="AS14" s="136"/>
-      <c r="AT14" s="136"/>
-      <c r="AU14" s="136"/>
-      <c r="AV14" s="136"/>
-      <c r="AW14" s="136"/>
-      <c r="AX14" s="136"/>
-      <c r="AY14" s="136"/>
-      <c r="AZ14" s="136"/>
-      <c r="BA14" s="136"/>
-      <c r="BB14" s="136"/>
-    </row>
-    <row r="15" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="125" t="s">
-        <v>291</v>
-      </c>
-      <c r="B15" s="125"/>
-      <c r="C15" s="130"/>
-      <c r="D15" s="133"/>
-      <c r="E15" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F15" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G15" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H15" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I15" s="125"/>
-      <c r="J15" s="125"/>
-      <c r="K15" s="130"/>
-      <c r="L15" s="133"/>
-      <c r="M15" s="125"/>
-      <c r="N15" s="125"/>
-      <c r="O15" s="130"/>
-      <c r="P15" s="133"/>
-      <c r="Q15" s="125"/>
-      <c r="R15" s="125"/>
-      <c r="S15" s="130"/>
-      <c r="T15" s="133"/>
-      <c r="U15" s="125"/>
-      <c r="V15" s="125"/>
-      <c r="W15" s="130"/>
-      <c r="X15" s="133"/>
-      <c r="Y15" s="125"/>
-      <c r="Z15" s="125"/>
-      <c r="AA15" s="130"/>
-      <c r="AB15" s="133"/>
-      <c r="AC15" s="125"/>
-      <c r="AD15" s="125"/>
-      <c r="AE15" s="130"/>
-      <c r="AF15" s="137"/>
-      <c r="AG15" s="135"/>
-      <c r="AH15" s="135"/>
-      <c r="AI15" s="135"/>
-      <c r="AJ15" s="136"/>
-      <c r="AK15" s="136"/>
-      <c r="AL15" s="136"/>
-      <c r="AM15" s="136"/>
-      <c r="AN15" s="136"/>
-      <c r="AO15" s="136"/>
-      <c r="AP15" s="136"/>
-      <c r="AQ15" s="136"/>
-      <c r="AR15" s="136"/>
-      <c r="AS15" s="136"/>
-      <c r="AT15" s="136"/>
-      <c r="AU15" s="136"/>
-      <c r="AV15" s="136"/>
-      <c r="AW15" s="136"/>
-      <c r="AX15" s="136"/>
-      <c r="AY15" s="136"/>
-      <c r="AZ15" s="136"/>
-      <c r="BA15" s="136"/>
-      <c r="BB15" s="136"/>
-    </row>
-    <row r="16" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="125" t="s">
-        <v>297</v>
-      </c>
-      <c r="B16" s="125"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F16" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G16" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H16" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I16" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J16" s="125"/>
-      <c r="K16" s="130"/>
-      <c r="L16" s="133"/>
-      <c r="M16" s="125"/>
-      <c r="N16" s="125"/>
-      <c r="O16" s="130"/>
-      <c r="P16" s="133"/>
-      <c r="Q16" s="125"/>
-      <c r="R16" s="125"/>
-      <c r="S16" s="130"/>
-      <c r="T16" s="133"/>
-      <c r="U16" s="125"/>
-      <c r="V16" s="125"/>
-      <c r="W16" s="130"/>
-      <c r="X16" s="133"/>
-      <c r="Y16" s="125"/>
-      <c r="Z16" s="125"/>
-      <c r="AA16" s="130"/>
-      <c r="AB16" s="133"/>
-      <c r="AC16" s="125"/>
-      <c r="AD16" s="125"/>
-      <c r="AE16" s="130"/>
-      <c r="AF16" s="137"/>
-      <c r="AG16" s="135"/>
-      <c r="AH16" s="135"/>
-      <c r="AI16" s="135"/>
-      <c r="AJ16" s="136"/>
-      <c r="AK16" s="136"/>
-      <c r="AL16" s="136"/>
-      <c r="AM16" s="136"/>
-      <c r="AN16" s="136"/>
-      <c r="AO16" s="136"/>
-      <c r="AP16" s="136"/>
-      <c r="AQ16" s="136"/>
-      <c r="AR16" s="136"/>
-      <c r="AS16" s="136"/>
-      <c r="AT16" s="136"/>
-      <c r="AU16" s="136"/>
-      <c r="AV16" s="136"/>
-      <c r="AW16" s="136"/>
-      <c r="AX16" s="136"/>
-      <c r="AY16" s="136"/>
-      <c r="AZ16" s="136"/>
-      <c r="BA16" s="136"/>
-      <c r="BB16" s="136"/>
-    </row>
-    <row r="17" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="125" t="s">
-        <v>293</v>
-      </c>
-      <c r="B17" s="125"/>
-      <c r="C17" s="130"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F17" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G17" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H17" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I17" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J17" s="125"/>
-      <c r="K17" s="130"/>
-      <c r="L17" s="133"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="125"/>
-      <c r="O17" s="130"/>
-      <c r="P17" s="133"/>
-      <c r="Q17" s="125"/>
-      <c r="R17" s="125"/>
-      <c r="S17" s="130"/>
-      <c r="T17" s="133"/>
-      <c r="U17" s="125"/>
-      <c r="V17" s="125"/>
-      <c r="W17" s="130"/>
-      <c r="X17" s="133"/>
-      <c r="Y17" s="125"/>
-      <c r="Z17" s="125"/>
-      <c r="AA17" s="130"/>
-      <c r="AB17" s="133"/>
-      <c r="AC17" s="125"/>
-      <c r="AD17" s="125"/>
-      <c r="AE17" s="130"/>
-      <c r="AF17" s="137"/>
-      <c r="AG17" s="135"/>
-      <c r="AH17" s="135"/>
-      <c r="AI17" s="135"/>
-      <c r="AJ17" s="136"/>
-      <c r="AK17" s="136"/>
-      <c r="AL17" s="136"/>
-      <c r="AM17" s="136"/>
-      <c r="AN17" s="136"/>
-      <c r="AO17" s="136"/>
-      <c r="AP17" s="136"/>
-      <c r="AQ17" s="136"/>
-      <c r="AR17" s="136"/>
-      <c r="AS17" s="136"/>
-      <c r="AT17" s="136"/>
-      <c r="AU17" s="136"/>
-      <c r="AV17" s="136"/>
-      <c r="AW17" s="136"/>
-      <c r="AX17" s="136"/>
-      <c r="AY17" s="136"/>
-      <c r="AZ17" s="136"/>
-      <c r="BA17" s="136"/>
-      <c r="BB17" s="136"/>
-    </row>
-    <row r="18" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="125" t="s">
-        <v>309</v>
-      </c>
-      <c r="B18" s="125"/>
-      <c r="C18" s="130"/>
-      <c r="D18" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="E18" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F18" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G18" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H18" s="133"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="125"/>
-      <c r="K18" s="130"/>
-      <c r="L18" s="133"/>
-      <c r="M18" s="125"/>
-      <c r="N18" s="125"/>
-      <c r="O18" s="130"/>
-      <c r="P18" s="133"/>
-      <c r="Q18" s="125"/>
-      <c r="R18" s="125"/>
-      <c r="S18" s="130"/>
-      <c r="T18" s="133"/>
-      <c r="U18" s="125"/>
-      <c r="V18" s="125"/>
-      <c r="W18" s="130"/>
-      <c r="X18" s="133"/>
-      <c r="Y18" s="125"/>
-      <c r="Z18" s="125"/>
-      <c r="AA18" s="130"/>
-      <c r="AB18" s="133"/>
-      <c r="AC18" s="125"/>
-      <c r="AD18" s="125"/>
-      <c r="AE18" s="130"/>
-      <c r="AF18" s="137"/>
-      <c r="AG18" s="135"/>
-      <c r="AH18" s="135"/>
-      <c r="AI18" s="135"/>
-      <c r="AJ18" s="136"/>
-      <c r="AK18" s="136"/>
-      <c r="AL18" s="136"/>
-      <c r="AM18" s="136"/>
-      <c r="AN18" s="136"/>
-      <c r="AO18" s="136"/>
-      <c r="AP18" s="136"/>
-      <c r="AQ18" s="136"/>
-      <c r="AR18" s="136"/>
-      <c r="AS18" s="136"/>
-      <c r="AT18" s="136"/>
-      <c r="AU18" s="136"/>
-      <c r="AV18" s="136"/>
-      <c r="AW18" s="136"/>
-      <c r="AX18" s="136"/>
-      <c r="AY18" s="136"/>
-      <c r="AZ18" s="136"/>
-      <c r="BA18" s="136"/>
-      <c r="BB18" s="136"/>
-    </row>
-    <row r="19" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="125" t="s">
+      <c r="B21" s="102"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="110" t="s">
         <v>294</v>
       </c>
-      <c r="B19" s="125"/>
-      <c r="C19" s="130"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F19" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G19" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H19" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I19" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J19" s="125"/>
-      <c r="K19" s="130"/>
-      <c r="L19" s="133"/>
-      <c r="M19" s="125"/>
-      <c r="N19" s="125"/>
-      <c r="O19" s="130"/>
-      <c r="P19" s="133"/>
-      <c r="Q19" s="125"/>
-      <c r="R19" s="125"/>
-      <c r="S19" s="130"/>
-      <c r="T19" s="133"/>
-      <c r="U19" s="125"/>
-      <c r="V19" s="125"/>
-      <c r="W19" s="130"/>
-      <c r="X19" s="133"/>
-      <c r="Y19" s="125"/>
-      <c r="Z19" s="125"/>
-      <c r="AA19" s="130"/>
-      <c r="AB19" s="133"/>
-      <c r="AC19" s="125"/>
-      <c r="AD19" s="125"/>
-      <c r="AE19" s="130"/>
-      <c r="AF19" s="137"/>
-      <c r="AG19" s="135"/>
-      <c r="AH19" s="135"/>
-      <c r="AI19" s="135"/>
-      <c r="AJ19" s="136"/>
-      <c r="AK19" s="136"/>
-      <c r="AL19" s="136"/>
-      <c r="AM19" s="136"/>
-      <c r="AN19" s="136"/>
-      <c r="AO19" s="136"/>
-      <c r="AP19" s="136"/>
-      <c r="AQ19" s="136"/>
-      <c r="AR19" s="136"/>
-      <c r="AS19" s="136"/>
-      <c r="AT19" s="136"/>
-      <c r="AU19" s="136"/>
-      <c r="AV19" s="136"/>
-      <c r="AW19" s="136"/>
-      <c r="AX19" s="136"/>
-      <c r="AY19" s="136"/>
-      <c r="AZ19" s="136"/>
-      <c r="BA19" s="136"/>
-      <c r="BB19" s="136"/>
-    </row>
-    <row r="20" spans="1:54" s="126" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="125" t="s">
-        <v>295</v>
-      </c>
-      <c r="B20" s="125"/>
-      <c r="C20" s="130"/>
-      <c r="D20" s="133"/>
-      <c r="E20" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="F20" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="G20" s="130" t="s">
-        <v>296</v>
-      </c>
-      <c r="H20" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I20" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J20" s="125"/>
-      <c r="K20" s="130"/>
-      <c r="L20" s="133"/>
-      <c r="M20" s="125"/>
-      <c r="N20" s="125"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="133"/>
-      <c r="Q20" s="125"/>
-      <c r="R20" s="125"/>
-      <c r="S20" s="130"/>
-      <c r="T20" s="133"/>
-      <c r="U20" s="125"/>
-      <c r="V20" s="125"/>
-      <c r="W20" s="130"/>
-      <c r="X20" s="133"/>
-      <c r="Y20" s="125"/>
-      <c r="Z20" s="125"/>
-      <c r="AA20" s="130"/>
-      <c r="AB20" s="133"/>
-      <c r="AC20" s="125"/>
-      <c r="AD20" s="125"/>
-      <c r="AE20" s="130"/>
-      <c r="AF20" s="137"/>
-      <c r="AG20" s="135"/>
-      <c r="AH20" s="135"/>
-      <c r="AI20" s="135"/>
-      <c r="AJ20" s="136"/>
-      <c r="AK20" s="136"/>
-      <c r="AL20" s="136"/>
-      <c r="AM20" s="136"/>
-      <c r="AN20" s="136"/>
-      <c r="AO20" s="136"/>
-      <c r="AP20" s="136"/>
-      <c r="AQ20" s="136"/>
-      <c r="AR20" s="136"/>
-      <c r="AS20" s="136"/>
-      <c r="AT20" s="136"/>
-      <c r="AU20" s="136"/>
-      <c r="AV20" s="136"/>
-      <c r="AW20" s="136"/>
-      <c r="AX20" s="136"/>
-      <c r="AY20" s="136"/>
-      <c r="AZ20" s="136"/>
-      <c r="BA20" s="136"/>
-      <c r="BB20" s="136"/>
-    </row>
-    <row r="21" spans="1:54" s="126" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="125" t="s">
-        <v>298</v>
-      </c>
-      <c r="B21" s="125"/>
-      <c r="C21" s="130"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="125"/>
-      <c r="F21" s="125"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="133" t="s">
-        <v>296</v>
-      </c>
-      <c r="I21" s="125" t="s">
-        <v>296</v>
-      </c>
-      <c r="J21" s="125"/>
-      <c r="K21" s="130"/>
-      <c r="L21" s="133"/>
-      <c r="M21" s="125"/>
-      <c r="N21" s="125"/>
-      <c r="O21" s="130"/>
-      <c r="P21" s="133"/>
-      <c r="Q21" s="125"/>
-      <c r="R21" s="125"/>
-      <c r="S21" s="130"/>
-      <c r="T21" s="133"/>
-      <c r="U21" s="125"/>
-      <c r="V21" s="125"/>
-      <c r="W21" s="130"/>
-      <c r="X21" s="133"/>
-      <c r="Y21" s="125"/>
-      <c r="Z21" s="125"/>
-      <c r="AA21" s="130"/>
-      <c r="AB21" s="133"/>
-      <c r="AC21" s="125"/>
-      <c r="AD21" s="125"/>
-      <c r="AE21" s="130"/>
-      <c r="AF21" s="137"/>
-      <c r="AG21" s="135"/>
-      <c r="AH21" s="135"/>
-      <c r="AI21" s="135"/>
-      <c r="AJ21" s="136"/>
-      <c r="AK21" s="136"/>
-      <c r="AL21" s="136"/>
-      <c r="AM21" s="136"/>
-      <c r="AN21" s="136"/>
-      <c r="AO21" s="136"/>
-      <c r="AP21" s="136"/>
-      <c r="AQ21" s="136"/>
-      <c r="AR21" s="136"/>
-      <c r="AS21" s="136"/>
-      <c r="AT21" s="136"/>
-      <c r="AU21" s="136"/>
-      <c r="AV21" s="136"/>
-      <c r="AW21" s="136"/>
-      <c r="AX21" s="136"/>
-      <c r="AY21" s="136"/>
-      <c r="AZ21" s="136"/>
-      <c r="BA21" s="136"/>
-      <c r="BB21" s="136"/>
+      <c r="I21" s="102" t="s">
+        <v>294</v>
+      </c>
+      <c r="J21" s="102"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="102"/>
+      <c r="N21" s="102"/>
+      <c r="O21" s="107"/>
+      <c r="P21" s="110"/>
+      <c r="Q21" s="102"/>
+      <c r="R21" s="102"/>
+      <c r="S21" s="107"/>
+      <c r="T21" s="110"/>
+      <c r="U21" s="102"/>
+      <c r="V21" s="102"/>
+      <c r="W21" s="107"/>
+      <c r="X21" s="110"/>
+      <c r="Y21" s="102"/>
+      <c r="Z21" s="102"/>
+      <c r="AA21" s="107"/>
+      <c r="AB21" s="110"/>
+      <c r="AC21" s="102"/>
+      <c r="AD21" s="102"/>
+      <c r="AE21" s="107"/>
+      <c r="AF21" s="114"/>
+      <c r="AG21" s="112"/>
+      <c r="AH21" s="112"/>
+      <c r="AI21" s="112"/>
+      <c r="AJ21" s="113"/>
+      <c r="AK21" s="113"/>
+      <c r="AL21" s="113"/>
+      <c r="AM21" s="113"/>
+      <c r="AN21" s="113"/>
+      <c r="AO21" s="113"/>
+      <c r="AP21" s="113"/>
+      <c r="AQ21" s="113"/>
+      <c r="AR21" s="113"/>
+      <c r="AS21" s="113"/>
+      <c r="AT21" s="113"/>
+      <c r="AU21" s="113"/>
+      <c r="AV21" s="113"/>
+      <c r="AW21" s="113"/>
+      <c r="AX21" s="113"/>
+      <c r="AY21" s="113"/>
+      <c r="AZ21" s="113"/>
+      <c r="BA21" s="113"/>
+      <c r="BB21" s="113"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>